<commit_message>
Updated RequestDB class, Added Project Status
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B896135-5FA1-4AA6-BA67-959AA819C3AA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB3D297-5416-41C2-A9B5-CCBFE3298492}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fromUser</t>
   </si>
@@ -44,21 +44,6 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>h</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>CHANGETITLE</t>
-  </si>
-  <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>s</t>
   </si>
 </sst>
 </file>
@@ -385,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -429,26 +414,6 @@
       </c>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Removed unnecessary SupervisorDB methods
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E4389F-89B4-438B-84AB-B01AE40B67DB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF9F4E4-A696-4D36-A33D-973E9537E270}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3732" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fromUser</t>
   </si>
@@ -44,25 +44,12 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>YCHERN</t>
-  </si>
-  <si>
-    <t>ASFLI</t>
-  </si>
-  <si>
-    <t>REGISTERPROJECT</t>
-  </si>
-  <si>
-    <t>PENDING</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -383,21 +370,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="2.77734375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5546875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.44140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.109375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.5546875"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -426,28 +413,6 @@
         <v>4</v>
       </c>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>13.0</v>
-      </c>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MAJOR Restructure to Entity Control Boundary
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CF9F4E4-A696-4D36-A33D-973E9537E270}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FF8AC9-B007-4BD6-BE86-BF527404BAAF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -373,7 +373,7 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A2" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Editted FYP_Coordinator, Added Manage Request
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FF8AC9-B007-4BD6-BE86-BF527404BAAF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DB3D297-5416-41C2-A9B5-CCBFE3298492}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fromUser</t>
   </si>
@@ -44,28 +44,12 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>YCHERN</t>
-  </si>
-  <si>
-    <t>ASFLI</t>
-  </si>
-  <si>
-    <t>REGISTERPROJECT</t>
-  </si>
-  <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>APPROVED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -386,21 +370,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD4"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="2.77734375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5546875"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.44140625"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.77734375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.109375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.5546875"/>
+    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -429,50 +413,6 @@
         <v>4</v>
       </c>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>16.0</v>
-      </c>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>15.0</v>
-      </c>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Limit No. Register Project Request feature
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="15">
   <si>
     <t>fromUser</t>
   </si>
@@ -44,12 +44,34 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>YCHERN</t>
+  </si>
+  <si>
+    <t>ASFLI</t>
+  </si>
+  <si>
+    <t>REGISTERPROJECT</t>
+  </si>
+  <si>
+    <t>PENDING</t>
+  </si>
+  <si>
+    <t>APPROVED</t>
+  </si>
+  <si>
+    <t>DEREGISTERPROJECT</t>
+  </si>
+  <si>
+    <t>CT113</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -370,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -378,13 +400,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="2.77734375"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5546875"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="12.44140625"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="8.77734375"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="8.109375"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.5546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -414,6 +436,248 @@
       </c>
       <c r="I1" s="1"/>
     </row>
+    <row r="2">
+      <c r="A2" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="B2" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F2" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="F3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G5" s="0"/>
+      <c r="H5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F7" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F8" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="G8" s="0"/>
+      <c r="H8" s="0"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F9" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="G9" s="0"/>
+      <c r="H9" s="0"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n" s="0">
+        <v>9.0</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F10" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F11" t="n" s="0">
+        <v>6.0</v>
+      </c>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n" s="0">
+        <v>11.0</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F12" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Limit No. Reg Req project feautre
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="15">
   <si>
     <t>fromUser</t>
   </si>
@@ -392,7 +392,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -678,6 +678,28 @@
       <c r="G12" s="0"/>
       <c r="H12" s="0"/>
     </row>
+    <row r="13">
+      <c r="A13" t="n" s="0">
+        <v>12.0</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F13" t="n" s="0">
+        <v>8.0</v>
+      </c>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Preparing to merge main
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="19">
   <si>
     <t>fromUser</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>ASJMZHENG</t>
+  </si>
+  <si>
+    <t>CHANGETITLE</t>
+  </si>
+  <si>
+    <t>tes</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -395,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
@@ -465,9 +474,7 @@
       <c r="A3" t="n" s="0">
         <v>2.0</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>13</v>
-      </c>
+      <c r="B3" s="0"/>
       <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
@@ -484,6 +491,76 @@
       <c r="H3" t="s" s="0">
         <v>15</v>
       </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F4" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F5" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="H5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="F6" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="H6" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added restrictions to num of proj
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10312"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6A8B2C-CEC4-8A4B-9D37-390012808D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B8416C-7DFF-CB42-92B8-60F3564C3EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fromUser</t>
   </si>
@@ -44,31 +44,12 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>YCHERN</t>
-  </si>
-  <si>
-    <t>ASFLI</t>
-  </si>
-  <si>
-    <t>REGISTERPROJECT</t>
-  </si>
-  <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>APPROVED</t>
-  </si>
-  <si>
-    <t>DEREGISTERPROJECT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,21 +370,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F3" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="2.83203125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.83203125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.1640625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.5"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -432,50 +413,6 @@
         <v>4</v>
       </c>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
edits for reg proj
</commit_message>
<xml_diff>
--- a/App/data/request_list.xlsx
+++ b/App/data/request_list.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92613886-7080-1343-B52C-DF4889CE44A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5224CAF6-3D56-314E-8F65-01E8AF32DA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="23260" windowHeight="12460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>fromUser</t>
   </si>
@@ -44,31 +44,12 @@
   </si>
   <si>
     <t>status</t>
-  </si>
-  <si>
-    <t>YCHERN</t>
-  </si>
-  <si>
-    <t>ASFLI</t>
-  </si>
-  <si>
-    <t>REGISTERPROJECT</t>
-  </si>
-  <si>
-    <t>PENDING</t>
-  </si>
-  <si>
-    <t>KOH1</t>
-  </si>
-  <si>
-    <t>CT113</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -389,21 +370,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="A2:H4"/>
+      <selection activeCell="A2" sqref="A2:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="2.83203125"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.5"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.5"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.6640625"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.83203125"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="8.1640625"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="13.5"/>
+    <col min="1" max="1" width="2.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -432,72 +413,6 @@
         <v>4</v>
       </c>
       <c r="I1" s="1"/>
-    </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F2" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F3" t="n" s="0">
-        <v>6.0</v>
-      </c>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>7.0</v>
-      </c>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>